<commit_message>
Rotten Tomatoes new test cases section 3
</commit_message>
<xml_diff>
--- a/src/test/resources/test_descriptions/RottenTomatoes_TestCases.xlsx
+++ b/src/test/resources/test_descriptions/RottenTomatoes_TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\project\UITest2Code\src\test\resources\test_descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BEF56C-361C-4CA5-A7AA-79D668E0A270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC66ADB7-160D-4991-8DEE-CC65CB3BAAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{791CFF3F-B61E-4861-A956-A2059CE938E6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="301">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -716,6 +716,225 @@
   </si>
   <si>
     <t>RT_36</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>RT_37</t>
+  </si>
+  <si>
+    <t>TV Shows Tab</t>
+  </si>
+  <si>
+    <t>Verify that after hovering over the TV shows top tab, a menu will get opened</t>
+  </si>
+  <si>
+    <t>1. Hover over the TV SHOWS tab</t>
+  </si>
+  <si>
+    <t>A menu will be displayed, with the titles NEW TV TONIGHT, MOST POPULAR TV ON RT, MORE, EPISODIC REVIEWS, CERTIFIED FRESH PICK</t>
+  </si>
+  <si>
+    <t>TV Shows - New TV Tonight - With Score</t>
+  </si>
+  <si>
+    <t>A menu will be displayed, with the title NEW TV TONIGHT. Under it there is a list of shows, some have a score, and some have no rating.</t>
+  </si>
+  <si>
+    <t>2. Click one of the shows with a score</t>
+  </si>
+  <si>
+    <t>RT_38</t>
+  </si>
+  <si>
+    <t>RT_39</t>
+  </si>
+  <si>
+    <t>2. Click one of the shows with no score</t>
+  </si>
+  <si>
+    <t>A movie's page will be displayed with the correct movie title and a no score message</t>
+  </si>
+  <si>
+    <t>TV Shows - New TV Tonight - View All</t>
+  </si>
+  <si>
+    <t>A menu will be displayed, with the title NEW TV TONIGHT.</t>
+  </si>
+  <si>
+    <t>2. Click the View All link under the title</t>
+  </si>
+  <si>
+    <t>Verify that clicking a show line from the new tv tonight category that has a score from the TV shows top tab works</t>
+  </si>
+  <si>
+    <t>Verify that clicking a show line from the new tv tonight category that has no score from the TV shows top tab works</t>
+  </si>
+  <si>
+    <t>RT_40</t>
+  </si>
+  <si>
+    <t>A page with the title NEW TV TONIGHT will be displayed. On the navigator column, the line New TV Tonight is active. The presented shows are sorted by tomatometer score.</t>
+  </si>
+  <si>
+    <t>A page with the title NEW TV TONIGHT will be displayed. The presented shows are sorted by tomatometer score.</t>
+  </si>
+  <si>
+    <t>TV Shows - New TV Tonight - View All - Change View</t>
+  </si>
+  <si>
+    <t>Verify that the changing view option in the New TV Tonight page is working</t>
+  </si>
+  <si>
+    <t>3. Click on the second view-icon</t>
+  </si>
+  <si>
+    <t>The shows will be displayed in a list-view and still sorted by score and the recently clicked butoon will become active.</t>
+  </si>
+  <si>
+    <t>4. Click on the first view-icon</t>
+  </si>
+  <si>
+    <t>The shows will not be displayed in a list-view and still sorted by score and the recently clicked butoon will become active.</t>
+  </si>
+  <si>
+    <t>RT_41</t>
+  </si>
+  <si>
+    <t>A menu will be displayed</t>
+  </si>
+  <si>
+    <t>2. Click the Top TV Shows link</t>
+  </si>
+  <si>
+    <t>A page with the title Top TV Shows will be displayed, including a carousel with items that change automatically</t>
+  </si>
+  <si>
+    <t>Verify that clicking the view all link of the new tv tonight category from the TV shows top tab works</t>
+  </si>
+  <si>
+    <t>RT_42</t>
+  </si>
+  <si>
+    <t>RT_43</t>
+  </si>
+  <si>
+    <t>TV Shows - Top TV Shows - Display</t>
+  </si>
+  <si>
+    <t>TV Shows - Top TV Shows - POPULAR SHOWS AVAILABLE ON STREAMING</t>
+  </si>
+  <si>
+    <t>3. Click the View All link at the bottom of POPULAR SHOWS AVAILABLE ON STREAMING</t>
+  </si>
+  <si>
+    <t>A page with the title Top TV Shows will be displayed, including a POPULAR SHOWS AVAILABLE ON STREAMING section with 7 media links</t>
+  </si>
+  <si>
+    <t>16 media links will be presented under the section</t>
+  </si>
+  <si>
+    <t>RT_44</t>
+  </si>
+  <si>
+    <t>A page with the title Top TV Shows will be displayed</t>
+  </si>
+  <si>
+    <t>3. Click the banner with the title PREMIERE DATES</t>
+  </si>
+  <si>
+    <t>A page with the title TV PREMIERE DATES 2021 will be presented. Under November title, there'll be dates of all the days in the month. Same for December.</t>
+  </si>
+  <si>
+    <t>TV Shows - Top TV Shows - Premiere Dates - Display</t>
+  </si>
+  <si>
+    <t>Verify that after clicking the Top TV Shows link in the TV Shows tab, its page is presented well</t>
+  </si>
+  <si>
+    <t>Verify that the View All function in POPULAR SHOWS AVAILABLE ON STREAMING section in Top TV Shows page works</t>
+  </si>
+  <si>
+    <t>Verify that Premiere Dates for TV shows page is presented well</t>
+  </si>
+  <si>
+    <t>RT_45</t>
+  </si>
+  <si>
+    <t>A page with the title TV PREMIERE DATES 2021 will be presented.</t>
+  </si>
+  <si>
+    <t>4. Click the November link</t>
+  </si>
+  <si>
+    <t>November title will be visible to the user</t>
+  </si>
+  <si>
+    <t>TV Shows - Top TV Shows - Premiere Dates - November Link</t>
+  </si>
+  <si>
+    <t>Verify that clicking a month link in Premiere Dates for TV shows page is working</t>
+  </si>
+  <si>
+    <t>TV PREMIERE DATES 2021 ARCHIVE page title will be displayed. January title will be visible to the user</t>
+  </si>
+  <si>
+    <t>4. Click the Archive January link</t>
+  </si>
+  <si>
+    <t>TV Shows - Top TV Shows - Premiere Dates - Archive Link</t>
+  </si>
+  <si>
+    <t>Verify that clicking an archive month link in Premiere Dates for TV shows page is working</t>
+  </si>
+  <si>
+    <t>RT_46</t>
+  </si>
+  <si>
+    <t>RT_47</t>
+  </si>
+  <si>
+    <t>4. Click the Renewed &amp; Cancelled link</t>
+  </si>
+  <si>
+    <t>TV Shows - Top TV Shows - Premiere Dates - Renewed &amp; Cancelled</t>
+  </si>
+  <si>
+    <t>RENEWED AND CANCELLED TV SHOWS 2021 page title will be displayed, with a letters menu (# A-Z).</t>
+  </si>
+  <si>
+    <t>5. Click the letter link 'G'</t>
+  </si>
+  <si>
+    <t>Verify that clicking the Renewed &amp; Cancelled link in Premiere Dates for TV shows page is working and the page functions well</t>
+  </si>
+  <si>
+    <t>The title 'G' will be visible. Under it there'll be a video and a list of shows. For each of them there will be a spesification - Renewed or Cancelled</t>
+  </si>
+  <si>
+    <t>6. Click the Back to Top link in the G section</t>
+  </si>
+  <si>
+    <t>The letters menu will become visible</t>
+  </si>
+  <si>
+    <t>RT_48</t>
+  </si>
+  <si>
+    <t>TV Shows - EPISODIC REVIEWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A menu will be displayed, with the title EPISODIC REVIEWS. </t>
+  </si>
+  <si>
+    <t>2. Click one of the links under the episodic reviews title</t>
+  </si>
+  <si>
+    <t>A movie's page will be displayed with the correct movie title. The subtitle EPISODES is visible.</t>
+  </si>
+  <si>
+    <t>Verify that clicking one of the episodic reviews links in the TV Shows tab, works well</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1384,6 +1603,9 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1423,42 +1645,57 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1474,22 +1711,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1806,10 +2028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B4C97A-71D1-473B-A994-4B6E5B9F3EEF}">
-  <dimension ref="A1:F114"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1842,26 +2064,26 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
     </row>
     <row r="3" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="50" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1872,10 +2094,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1884,16 +2106,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="3"/>
@@ -1902,10 +2124,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="52"/>
+      <c r="A6" s="57"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="58"/>
       <c r="E6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1914,16 +2136,16 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="50" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3"/>
@@ -1932,10 +2154,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="49"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="55"/>
-      <c r="D8" s="43"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="51"/>
       <c r="E8" s="13" t="s">
         <v>21</v>
       </c>
@@ -1944,10 +2166,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="55"/>
-      <c r="D9" s="43"/>
+      <c r="A9" s="59"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="10" t="s">
         <v>23</v>
       </c>
@@ -1956,16 +2178,16 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="12" t="s">
@@ -1974,10 +2196,10 @@
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="43"/>
+      <c r="A11" s="56"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="51"/>
       <c r="E11" s="13" t="s">
         <v>39</v>
       </c>
@@ -1986,16 +2208,16 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -2006,10 +2228,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="59"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="43"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="51"/>
       <c r="E13" s="13" t="s">
         <v>42</v>
       </c>
@@ -2018,16 +2240,16 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -2038,10 +2260,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A15" s="60"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="43"/>
+      <c r="A15" s="62"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="15" t="s">
         <v>53</v>
       </c>
@@ -2050,10 +2272,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="43"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="15" t="s">
         <v>55</v>
       </c>
@@ -2062,16 +2284,16 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="12"/>
@@ -2080,10 +2302,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="59"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="43"/>
+      <c r="A18" s="53"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="13" t="s">
         <v>70</v>
       </c>
@@ -2092,10 +2314,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="52"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="58"/>
       <c r="E19" s="11" t="s">
         <v>71</v>
       </c>
@@ -2124,16 +2346,16 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="12"/>
@@ -2142,10 +2364,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="61"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="45"/>
       <c r="E22" s="13" t="s">
         <v>62</v>
       </c>
@@ -2154,26 +2376,26 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="61"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="16"/>
       <c r="F23" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="12" t="s">
@@ -2184,26 +2406,26 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="8"/>
       <c r="F25" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="12" t="s">
@@ -2214,10 +2436,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="37"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="8" t="s">
         <v>77</v>
       </c>
@@ -2226,16 +2448,16 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -2246,10 +2468,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
-      <c r="B29" s="41"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="36"/>
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="16" t="s">
         <v>82</v>
       </c>
@@ -2258,10 +2480,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="37"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="8" t="s">
         <v>84</v>
       </c>
@@ -2270,16 +2492,16 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="12" t="s">
@@ -2290,10 +2512,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A32" s="39"/>
-      <c r="B32" s="41"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="36"/>
+      <c r="A32" s="43"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="16" t="s">
         <v>82</v>
       </c>
@@ -2302,10 +2524,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
-      <c r="B33" s="47"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="37"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="38"/>
       <c r="E33" s="8" t="s">
         <v>87</v>
       </c>
@@ -2314,16 +2536,16 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="B34" s="40" t="s">
+      <c r="B34" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="12" t="s">
@@ -2332,10 +2554,10 @@
       <c r="F34" s="17"/>
     </row>
     <row r="35" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="37"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="8" t="s">
         <v>94</v>
       </c>
@@ -2344,16 +2566,16 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="32" t="s">
+      <c r="C36" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E36" s="12" t="s">
@@ -2364,26 +2586,26 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="47"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="37"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="42"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="8"/>
       <c r="F37" s="9" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="41" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E38" s="12" t="s">
@@ -2394,10 +2616,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="66.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="46"/>
-      <c r="B39" s="47"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="37"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="8" t="s">
         <v>106</v>
       </c>
@@ -2406,16 +2628,16 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="C40" s="32" t="s">
+      <c r="C40" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E40" s="12" t="s">
@@ -2426,10 +2648,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="46"/>
-      <c r="B41" s="47"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="37"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="38"/>
       <c r="E41" s="8" t="s">
         <v>109</v>
       </c>
@@ -2458,16 +2680,16 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="50.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="C43" s="32" t="s">
+      <c r="C43" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="12" t="s">
@@ -2478,10 +2700,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="46"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="37"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="38"/>
       <c r="E44" s="8" t="s">
         <v>121</v>
       </c>
@@ -2490,16 +2712,16 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="C45" s="32" t="s">
+      <c r="C45" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E45" s="12" t="s">
@@ -2510,10 +2732,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="46"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="37"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="38"/>
       <c r="E46" s="8" t="s">
         <v>106</v>
       </c>
@@ -2522,14 +2744,14 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
     </row>
     <row r="48" spans="1:6" ht="51" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
@@ -2552,16 +2774,16 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="33.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="32" t="s">
+      <c r="C49" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E49" s="16" t="s">
@@ -2572,10 +2794,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="46"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="37"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="38"/>
       <c r="E50" s="8" t="s">
         <v>133</v>
       </c>
@@ -2584,16 +2806,16 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="B51" s="40" t="s">
+      <c r="B51" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="C51" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E51" s="16" t="s">
@@ -2604,10 +2826,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="83.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
-      <c r="B52" s="47"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="37"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="38"/>
       <c r="E52" s="8" t="s">
         <v>137</v>
       </c>
@@ -2616,16 +2838,16 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="C53" s="32" t="s">
+      <c r="C53" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="D53" s="35" t="s">
+      <c r="D53" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E53" s="16" t="s">
@@ -2636,10 +2858,10 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="36"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="25" t="s">
         <v>137</v>
       </c>
@@ -2648,10 +2870,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="34"/>
-      <c r="D55" s="37"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="38"/>
       <c r="E55" s="8" t="s">
         <v>144</v>
       </c>
@@ -2660,16 +2882,16 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="26" t="s">
+      <c r="A56" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="35" t="s">
+      <c r="D56" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E56" s="16" t="s">
@@ -2680,10 +2902,10 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A57" s="27"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="36"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="25" t="s">
         <v>137</v>
       </c>
@@ -2692,10 +2914,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A58" s="27"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="36"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="25" t="s">
         <v>144</v>
       </c>
@@ -2704,10 +2926,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="27"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="36"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="25" t="s">
         <v>148</v>
       </c>
@@ -2716,10 +2938,10 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="37"/>
+      <c r="A60" s="29"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="38"/>
       <c r="E60" s="8" t="s">
         <v>150</v>
       </c>
@@ -2728,16 +2950,16 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="26" t="s">
+      <c r="A61" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="B61" s="29" t="s">
+      <c r="B61" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="D61" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E61" s="16" t="s">
@@ -2748,10 +2970,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A62" s="27"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="36"/>
+      <c r="A62" s="28"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="25" t="s">
         <v>137</v>
       </c>
@@ -2760,10 +2982,10 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A63" s="27"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="36"/>
+      <c r="A63" s="28"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="25" t="s">
         <v>144</v>
       </c>
@@ -2772,10 +2994,10 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="99" x14ac:dyDescent="0.2">
-      <c r="A64" s="27"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="36"/>
+      <c r="A64" s="28"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="25" t="s">
         <v>161</v>
       </c>
@@ -2784,10 +3006,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="28"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="37"/>
+      <c r="A65" s="29"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="38"/>
       <c r="E65" s="8" t="s">
         <v>163</v>
       </c>
@@ -2796,16 +3018,16 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="26" t="s">
+      <c r="A66" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="B66" s="29" t="s">
+      <c r="B66" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="C66" s="32" t="s">
+      <c r="C66" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="D66" s="35" t="s">
+      <c r="D66" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E66" s="16" t="s">
@@ -2816,10 +3038,10 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A67" s="27"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="36"/>
+      <c r="A67" s="28"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="25" t="s">
         <v>172</v>
       </c>
@@ -2828,10 +3050,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A68" s="27"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="33"/>
-      <c r="D68" s="36"/>
+      <c r="A68" s="28"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="37"/>
       <c r="E68" s="25" t="s">
         <v>174</v>
       </c>
@@ -2840,10 +3062,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="28"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="37"/>
+      <c r="A69" s="29"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="35"/>
+      <c r="D69" s="38"/>
       <c r="E69" s="8" t="s">
         <v>177</v>
       </c>
@@ -2852,16 +3074,16 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="26" t="s">
+      <c r="A70" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="C70" s="32" t="s">
+      <c r="C70" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="D70" s="35" t="s">
+      <c r="D70" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E70" s="16" t="s">
@@ -2872,10 +3094,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A71" s="27"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="36"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="37"/>
       <c r="E71" s="25" t="s">
         <v>172</v>
       </c>
@@ -2884,10 +3106,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="28"/>
-      <c r="B72" s="31"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="37"/>
+      <c r="A72" s="29"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="38"/>
       <c r="E72" s="8" t="s">
         <v>182</v>
       </c>
@@ -2896,16 +3118,16 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="33.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="38" t="s">
+      <c r="A73" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="B73" s="40" t="s">
+      <c r="B73" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="C73" s="32" t="s">
+      <c r="C73" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="D73" s="42" t="s">
+      <c r="D73" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E73" s="16" t="s">
@@ -2916,10 +3138,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="39"/>
-      <c r="B74" s="41"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="43"/>
+      <c r="A74" s="43"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="51"/>
       <c r="E74" s="25" t="s">
         <v>172</v>
       </c>
@@ -2928,10 +3150,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A75" s="39"/>
-      <c r="B75" s="41"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="43"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="51"/>
       <c r="E75" s="25" t="s">
         <v>205</v>
       </c>
@@ -2940,10 +3162,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="39"/>
-      <c r="B76" s="41"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="43"/>
+      <c r="A76" s="43"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="51"/>
       <c r="E76" s="8" t="s">
         <v>206</v>
       </c>
@@ -2952,16 +3174,16 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="26" t="s">
+      <c r="A77" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="B77" s="29" t="s">
+      <c r="B77" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="C77" s="32" t="s">
+      <c r="C77" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="D77" s="35" t="s">
+      <c r="D77" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E77" s="16" t="s">
@@ -2972,20 +3194,20 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A78" s="27"/>
-      <c r="B78" s="30"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="36"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F78" s="6"/>
     </row>
     <row r="79" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A79" s="27"/>
-      <c r="B79" s="30"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="36"/>
+      <c r="A79" s="28"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="25" t="s">
         <v>185</v>
       </c>
@@ -2994,10 +3216,10 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="66.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="28"/>
-      <c r="B80" s="31"/>
-      <c r="C80" s="34"/>
-      <c r="D80" s="37"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="38"/>
       <c r="E80" s="8" t="s">
         <v>186</v>
       </c>
@@ -3006,16 +3228,16 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="B81" s="29" t="s">
+      <c r="B81" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="C81" s="32" t="s">
+      <c r="C81" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="D81" s="35" t="s">
+      <c r="D81" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E81" s="16" t="s">
@@ -3026,20 +3248,20 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="27"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="36"/>
+      <c r="A82" s="28"/>
+      <c r="B82" s="31"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="37"/>
       <c r="E82" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F82" s="6"/>
     </row>
     <row r="83" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A83" s="27"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="33"/>
-      <c r="D83" s="36"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="31"/>
+      <c r="C83" s="34"/>
+      <c r="D83" s="37"/>
       <c r="E83" s="25" t="s">
         <v>185</v>
       </c>
@@ -3048,10 +3270,10 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A84" s="27"/>
-      <c r="B84" s="30"/>
-      <c r="C84" s="33"/>
-      <c r="D84" s="36"/>
+      <c r="A84" s="28"/>
+      <c r="B84" s="31"/>
+      <c r="C84" s="34"/>
+      <c r="D84" s="37"/>
       <c r="E84" s="16" t="s">
         <v>186</v>
       </c>
@@ -3060,10 +3282,10 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
-      <c r="B85" s="31"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="37"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="35"/>
+      <c r="D85" s="38"/>
       <c r="E85" s="8" t="s">
         <v>209</v>
       </c>
@@ -3072,16 +3294,16 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="26" t="s">
+      <c r="A86" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="B86" s="29" t="s">
+      <c r="B86" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="C86" s="32" t="s">
+      <c r="C86" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="D86" s="35" t="s">
+      <c r="D86" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E86" s="16" t="s">
@@ -3092,20 +3314,20 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A87" s="27"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="33"/>
-      <c r="D87" s="36"/>
+      <c r="A87" s="28"/>
+      <c r="B87" s="31"/>
+      <c r="C87" s="34"/>
+      <c r="D87" s="37"/>
       <c r="E87" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F87" s="6"/>
     </row>
     <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A88" s="27"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="33"/>
-      <c r="D88" s="36"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="31"/>
+      <c r="C88" s="34"/>
+      <c r="D88" s="37"/>
       <c r="E88" s="25" t="s">
         <v>185</v>
       </c>
@@ -3114,10 +3336,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A89" s="27"/>
-      <c r="B89" s="30"/>
-      <c r="C89" s="33"/>
-      <c r="D89" s="36"/>
+      <c r="A89" s="28"/>
+      <c r="B89" s="31"/>
+      <c r="C89" s="34"/>
+      <c r="D89" s="37"/>
       <c r="E89" s="16" t="s">
         <v>186</v>
       </c>
@@ -3126,10 +3348,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
-      <c r="B90" s="31"/>
-      <c r="C90" s="34"/>
-      <c r="D90" s="37"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="35"/>
+      <c r="D90" s="38"/>
       <c r="E90" s="8" t="s">
         <v>196</v>
       </c>
@@ -3138,16 +3360,16 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="26" t="s">
+      <c r="A91" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="B91" s="29" t="s">
+      <c r="B91" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="C91" s="32" t="s">
+      <c r="C91" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="D91" s="35" t="s">
+      <c r="D91" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E91" s="16" t="s">
@@ -3158,20 +3380,20 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="27"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="33"/>
-      <c r="D92" s="36"/>
+      <c r="A92" s="28"/>
+      <c r="B92" s="31"/>
+      <c r="C92" s="34"/>
+      <c r="D92" s="37"/>
       <c r="E92" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F92" s="6"/>
     </row>
     <row r="93" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A93" s="27"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="33"/>
-      <c r="D93" s="36"/>
+      <c r="A93" s="28"/>
+      <c r="B93" s="31"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="37"/>
       <c r="E93" s="25" t="s">
         <v>185</v>
       </c>
@@ -3180,10 +3402,10 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A94" s="27"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="33"/>
-      <c r="D94" s="36"/>
+      <c r="A94" s="28"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="34"/>
+      <c r="D94" s="37"/>
       <c r="E94" s="16" t="s">
         <v>186</v>
       </c>
@@ -3192,10 +3414,10 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
-      <c r="B95" s="31"/>
-      <c r="C95" s="34"/>
-      <c r="D95" s="37"/>
+      <c r="A95" s="29"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="35"/>
+      <c r="D95" s="38"/>
       <c r="E95" s="8" t="s">
         <v>215</v>
       </c>
@@ -3204,16 +3426,16 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="26" t="s">
+      <c r="A96" s="27" t="s">
         <v>210</v>
       </c>
-      <c r="B96" s="29" t="s">
+      <c r="B96" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="C96" s="32" t="s">
+      <c r="C96" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="D96" s="35" t="s">
+      <c r="D96" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E96" s="16" t="s">
@@ -3224,20 +3446,20 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="27"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="33"/>
-      <c r="D97" s="36"/>
+      <c r="A97" s="28"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="34"/>
+      <c r="D97" s="37"/>
       <c r="E97" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F97" s="6"/>
     </row>
     <row r="98" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A98" s="27"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="33"/>
-      <c r="D98" s="36"/>
+      <c r="A98" s="28"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="37"/>
       <c r="E98" s="25" t="s">
         <v>185</v>
       </c>
@@ -3246,10 +3468,10 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A99" s="27"/>
-      <c r="B99" s="30"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="36"/>
+      <c r="A99" s="28"/>
+      <c r="B99" s="31"/>
+      <c r="C99" s="34"/>
+      <c r="D99" s="37"/>
       <c r="E99" s="16" t="s">
         <v>186</v>
       </c>
@@ -3258,10 +3480,10 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
-      <c r="B100" s="31"/>
-      <c r="C100" s="34"/>
-      <c r="D100" s="37"/>
+      <c r="A100" s="29"/>
+      <c r="B100" s="32"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="38"/>
       <c r="E100" s="8" t="s">
         <v>214</v>
       </c>
@@ -3270,16 +3492,16 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="26" t="s">
+      <c r="A101" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C101" s="32" t="s">
+      <c r="C101" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="D101" s="35" t="s">
+      <c r="D101" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E101" s="16" t="s">
@@ -3290,20 +3512,20 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A102" s="27"/>
-      <c r="B102" s="30"/>
-      <c r="C102" s="33"/>
-      <c r="D102" s="36"/>
+      <c r="A102" s="28"/>
+      <c r="B102" s="31"/>
+      <c r="C102" s="34"/>
+      <c r="D102" s="37"/>
       <c r="E102" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F102" s="6"/>
     </row>
     <row r="103" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A103" s="27"/>
-      <c r="B103" s="30"/>
-      <c r="C103" s="33"/>
-      <c r="D103" s="36"/>
+      <c r="A103" s="28"/>
+      <c r="B103" s="31"/>
+      <c r="C103" s="34"/>
+      <c r="D103" s="37"/>
       <c r="E103" s="25" t="s">
         <v>185</v>
       </c>
@@ -3312,10 +3534,10 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A104" s="27"/>
-      <c r="B104" s="30"/>
-      <c r="C104" s="33"/>
-      <c r="D104" s="36"/>
+      <c r="A104" s="28"/>
+      <c r="B104" s="31"/>
+      <c r="C104" s="34"/>
+      <c r="D104" s="37"/>
       <c r="E104" s="25" t="s">
         <v>186</v>
       </c>
@@ -3324,10 +3546,10 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A105" s="27"/>
-      <c r="B105" s="30"/>
-      <c r="C105" s="33"/>
-      <c r="D105" s="36"/>
+      <c r="A105" s="28"/>
+      <c r="B105" s="31"/>
+      <c r="C105" s="34"/>
+      <c r="D105" s="37"/>
       <c r="E105" s="25" t="s">
         <v>214</v>
       </c>
@@ -3336,10 +3558,10 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="28"/>
-      <c r="B106" s="31"/>
-      <c r="C106" s="34"/>
-      <c r="D106" s="37"/>
+      <c r="A106" s="29"/>
+      <c r="B106" s="32"/>
+      <c r="C106" s="35"/>
+      <c r="D106" s="38"/>
       <c r="E106" s="8" t="s">
         <v>216</v>
       </c>
@@ -3348,16 +3570,16 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="26" t="s">
+      <c r="A107" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="B107" s="29" t="s">
+      <c r="B107" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="C107" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="D107" s="35" t="s">
+      <c r="D107" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E107" s="16" t="s">
@@ -3368,20 +3590,20 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A108" s="27"/>
-      <c r="B108" s="30"/>
-      <c r="C108" s="33"/>
-      <c r="D108" s="36"/>
+      <c r="A108" s="28"/>
+      <c r="B108" s="31"/>
+      <c r="C108" s="34"/>
+      <c r="D108" s="37"/>
       <c r="E108" s="25" t="s">
         <v>172</v>
       </c>
       <c r="F108" s="6"/>
     </row>
     <row r="109" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A109" s="27"/>
-      <c r="B109" s="30"/>
-      <c r="C109" s="33"/>
-      <c r="D109" s="36"/>
+      <c r="A109" s="28"/>
+      <c r="B109" s="31"/>
+      <c r="C109" s="34"/>
+      <c r="D109" s="37"/>
       <c r="E109" s="25" t="s">
         <v>185</v>
       </c>
@@ -3390,10 +3612,10 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A110" s="27"/>
-      <c r="B110" s="30"/>
-      <c r="C110" s="33"/>
-      <c r="D110" s="36"/>
+      <c r="A110" s="28"/>
+      <c r="B110" s="31"/>
+      <c r="C110" s="34"/>
+      <c r="D110" s="37"/>
       <c r="E110" s="25" t="s">
         <v>186</v>
       </c>
@@ -3402,10 +3624,10 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A111" s="27"/>
-      <c r="B111" s="30"/>
-      <c r="C111" s="33"/>
-      <c r="D111" s="36"/>
+      <c r="A111" s="28"/>
+      <c r="B111" s="31"/>
+      <c r="C111" s="34"/>
+      <c r="D111" s="37"/>
       <c r="E111" s="25" t="s">
         <v>214</v>
       </c>
@@ -3414,10 +3636,10 @@
       </c>
     </row>
     <row r="112" spans="1:6" ht="33" x14ac:dyDescent="0.2">
-      <c r="A112" s="27"/>
-      <c r="B112" s="30"/>
-      <c r="C112" s="33"/>
-      <c r="D112" s="36"/>
+      <c r="A112" s="28"/>
+      <c r="B112" s="31"/>
+      <c r="C112" s="34"/>
+      <c r="D112" s="37"/>
       <c r="E112" s="16" t="s">
         <v>218</v>
       </c>
@@ -3426,10 +3648,10 @@
       </c>
     </row>
     <row r="113" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="28"/>
-      <c r="B113" s="31"/>
-      <c r="C113" s="34"/>
-      <c r="D113" s="37"/>
+      <c r="A113" s="29"/>
+      <c r="B113" s="32"/>
+      <c r="C113" s="35"/>
+      <c r="D113" s="38"/>
       <c r="E113" s="8" t="s">
         <v>220</v>
       </c>
@@ -3437,21 +3659,678 @@
         <v>221</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="114" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="46" t="s">
+        <v>228</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="47"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+    </row>
+    <row r="115" spans="1:6" ht="51" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="B115" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C115" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="D115" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="50.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="39" t="s">
+        <v>237</v>
+      </c>
+      <c r="B116" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="C116" s="33" t="s">
+        <v>244</v>
+      </c>
+      <c r="D116" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F116" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="40"/>
+      <c r="B117" s="42"/>
+      <c r="C117" s="35"/>
+      <c r="D117" s="38"/>
+      <c r="E117" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="50.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="C118" s="33" t="s">
+        <v>245</v>
+      </c>
+      <c r="D118" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F118" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="40"/>
+      <c r="B119" s="42"/>
+      <c r="C119" s="35"/>
+      <c r="D119" s="38"/>
+      <c r="E119" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="39" t="s">
+        <v>246</v>
+      </c>
+      <c r="B120" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="D120" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F120" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="40"/>
+      <c r="B121" s="42"/>
+      <c r="C121" s="35"/>
+      <c r="D121" s="38"/>
+      <c r="E121" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="B122" s="41" t="s">
+        <v>249</v>
+      </c>
+      <c r="C122" s="33" t="s">
+        <v>250</v>
+      </c>
+      <c r="D122" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F122" s="17" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A123" s="43"/>
+      <c r="B123" s="44"/>
+      <c r="C123" s="34"/>
+      <c r="D123" s="37"/>
+      <c r="E123" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A124" s="43"/>
+      <c r="B124" s="44"/>
+      <c r="C124" s="34"/>
+      <c r="D124" s="37"/>
+      <c r="E124" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="40"/>
+      <c r="B125" s="42"/>
+      <c r="C125" s="35"/>
+      <c r="D125" s="38"/>
+      <c r="E125" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="F125" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="39" t="s">
+        <v>260</v>
+      </c>
+      <c r="B126" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="C126" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="D126" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E126" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F126" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="40"/>
+      <c r="B127" s="42"/>
+      <c r="C127" s="35"/>
+      <c r="D127" s="38"/>
+      <c r="E127" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="39" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" s="41" t="s">
+        <v>263</v>
+      </c>
+      <c r="C128" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D128" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F128" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A129" s="43"/>
+      <c r="B129" s="44"/>
+      <c r="C129" s="34"/>
+      <c r="D129" s="37"/>
+      <c r="E129" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="40"/>
+      <c r="B130" s="42"/>
+      <c r="C130" s="35"/>
+      <c r="D130" s="38"/>
+      <c r="E130" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="B131" s="41" t="s">
+        <v>271</v>
+      </c>
+      <c r="C131" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="D131" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E131" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F131" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A132" s="43"/>
+      <c r="B132" s="44"/>
+      <c r="C132" s="34"/>
+      <c r="D132" s="37"/>
+      <c r="E132" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="50.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="40"/>
+      <c r="B133" s="42"/>
+      <c r="C133" s="35"/>
+      <c r="D133" s="38"/>
+      <c r="E133" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="F133" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="39" t="s">
+        <v>275</v>
+      </c>
+      <c r="B134" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C134" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="D134" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E134" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F134" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A135" s="43"/>
+      <c r="B135" s="44"/>
+      <c r="C135" s="34"/>
+      <c r="D135" s="37"/>
+      <c r="E135" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A136" s="43"/>
+      <c r="B136" s="44"/>
+      <c r="C136" s="34"/>
+      <c r="D136" s="37"/>
+      <c r="E136" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="40"/>
+      <c r="B137" s="42"/>
+      <c r="C137" s="35"/>
+      <c r="D137" s="38"/>
+      <c r="E137" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="F137" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="B138" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C138" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="D138" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E138" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F138" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A139" s="43"/>
+      <c r="B139" s="44"/>
+      <c r="C139" s="34"/>
+      <c r="D139" s="37"/>
+      <c r="E139" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A140" s="43"/>
+      <c r="B140" s="44"/>
+      <c r="C140" s="34"/>
+      <c r="D140" s="37"/>
+      <c r="E140" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="40"/>
+      <c r="B141" s="42"/>
+      <c r="C141" s="35"/>
+      <c r="D141" s="38"/>
+      <c r="E141" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="F141" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="39" t="s">
+        <v>286</v>
+      </c>
+      <c r="B142" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="C142" s="33" t="s">
+        <v>291</v>
+      </c>
+      <c r="D142" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F142" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A143" s="43"/>
+      <c r="B143" s="44"/>
+      <c r="C143" s="34"/>
+      <c r="D143" s="37"/>
+      <c r="E143" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A144" s="43"/>
+      <c r="B144" s="44"/>
+      <c r="C144" s="34"/>
+      <c r="D144" s="37"/>
+      <c r="E144" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="F144" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+      <c r="A145" s="43"/>
+      <c r="B145" s="44"/>
+      <c r="C145" s="34"/>
+      <c r="D145" s="37"/>
+      <c r="E145" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+      <c r="A146" s="43"/>
+      <c r="B146" s="44"/>
+      <c r="C146" s="34"/>
+      <c r="D146" s="37"/>
+      <c r="E146" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="F146" s="6" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="40"/>
+      <c r="B147" s="42"/>
+      <c r="C147" s="35"/>
+      <c r="D147" s="38"/>
+      <c r="E147" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="F147" s="9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" ht="17.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B148" s="41" t="s">
+        <v>296</v>
+      </c>
+      <c r="C148" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="D148" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="F148" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" ht="33.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="40"/>
+      <c r="B149" s="42"/>
+      <c r="C149" s="35"/>
+      <c r="D149" s="38"/>
+      <c r="E149" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="F149" s="9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="134">
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="C96:C100"/>
-    <mergeCell ref="D96:D100"/>
-    <mergeCell ref="A101:A106"/>
-    <mergeCell ref="B101:B106"/>
-    <mergeCell ref="C101:C106"/>
-    <mergeCell ref="D101:D106"/>
-    <mergeCell ref="A107:A113"/>
-    <mergeCell ref="B107:B113"/>
-    <mergeCell ref="C107:C113"/>
-    <mergeCell ref="D107:D113"/>
+  <mergeCells count="179">
+    <mergeCell ref="A138:A141"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="C138:C141"/>
+    <mergeCell ref="D138:D141"/>
+    <mergeCell ref="A142:A147"/>
+    <mergeCell ref="B142:B147"/>
+    <mergeCell ref="C142:C147"/>
+    <mergeCell ref="D142:D147"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="C148:C149"/>
+    <mergeCell ref="D148:D149"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="C128:C130"/>
+    <mergeCell ref="D128:D130"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="D131:D133"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="C134:C137"/>
+    <mergeCell ref="D134:D137"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="C120:C121"/>
+    <mergeCell ref="D120:D121"/>
+    <mergeCell ref="A122:A125"/>
+    <mergeCell ref="B122:B125"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="C126:C127"/>
+    <mergeCell ref="D126:D127"/>
+    <mergeCell ref="A114:F114"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="C118:C119"/>
+    <mergeCell ref="D118:D119"/>
+    <mergeCell ref="A86:A90"/>
+    <mergeCell ref="B86:B90"/>
+    <mergeCell ref="C86:C90"/>
+    <mergeCell ref="D86:D90"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="C91:C95"/>
+    <mergeCell ref="D91:D95"/>
+    <mergeCell ref="A81:A85"/>
+    <mergeCell ref="B81:B85"/>
+    <mergeCell ref="C81:C85"/>
+    <mergeCell ref="D81:D85"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="B77:B80"/>
+    <mergeCell ref="C77:C80"/>
+    <mergeCell ref="D77:D80"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="C73:C76"/>
+    <mergeCell ref="D73:D76"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="D70:D72"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="C56:C60"/>
+    <mergeCell ref="D56:D60"/>
+    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A38:A39"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="B40:B41"/>
@@ -3472,108 +4351,22 @@
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="A56:A60"/>
     <mergeCell ref="B56:B60"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
     <mergeCell ref="D45:D46"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C56:C60"/>
-    <mergeCell ref="D56:D60"/>
-    <mergeCell ref="A47:F47"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="C77:C80"/>
-    <mergeCell ref="D77:D80"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="C73:C76"/>
-    <mergeCell ref="D73:D76"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="C70:C72"/>
-    <mergeCell ref="D70:D72"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="B86:B90"/>
-    <mergeCell ref="C86:C90"/>
-    <mergeCell ref="D86:D90"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="C91:C95"/>
-    <mergeCell ref="D91:D95"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="B81:B85"/>
-    <mergeCell ref="C81:C85"/>
-    <mergeCell ref="D81:D85"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="C96:C100"/>
+    <mergeCell ref="D96:D100"/>
+    <mergeCell ref="A101:A106"/>
+    <mergeCell ref="B101:B106"/>
+    <mergeCell ref="C101:C106"/>
+    <mergeCell ref="D101:D106"/>
+    <mergeCell ref="A107:A113"/>
+    <mergeCell ref="B107:B113"/>
+    <mergeCell ref="C107:C113"/>
+    <mergeCell ref="D107:D113"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>

</xml_diff>